<commit_message>
Add support for create zip files in output, add samples, minor changes, in progress...
</commit_message>
<xml_diff>
--- a/src/samples/NetCore/iXlsxWriter.ConsoleAppCore/Output/Sample-01/Sample-01.xlsx
+++ b/src/samples/NetCore/iXlsxWriter.ConsoleAppCore/Output/Sample-01/Sample-01.xlsx
@@ -70,8 +70,8 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="3ranmjdc" xfId="1"/>
-    <cellStyle name="3ranmjdc_Alternate" xfId="2"/>
+    <cellStyle name="lohyc1gx" xfId="1"/>
+    <cellStyle name="lohyc1gx_Alternate" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
 </styleSheet>

</xml_diff>

<commit_message>
Add more samples, minor changes, in progress...
</commit_message>
<xml_diff>
--- a/src/samples/NetCore/iXlsxWriter.ConsoleAppCore/Output/Sample-01/Sample-01.xlsx
+++ b/src/samples/NetCore/iXlsxWriter.ConsoleAppCore/Output/Sample-01/Sample-01.xlsx
@@ -60,7 +60,7 @@
     </xf>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" xfId="0" applyProtection="1"/>
     <xf numFmtId="49" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" xfId="1" applyProtection="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -70,8 +70,8 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="lohyc1gx" xfId="1"/>
-    <cellStyle name="lohyc1gx_Alternate" xfId="2"/>
+    <cellStyle name="ez45dejw" xfId="1"/>
+    <cellStyle name="ez45dejw_Alternate" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
 </styleSheet>
@@ -91,8 +91,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.787400" right="0.787400" top="0.787400" bottom="0.787400" header="0.315" footer="0.315"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>